<commit_message>
kod za plotvane i excel tablica
</commit_message>
<xml_diff>
--- a/XFoil_Data.xlsx
+++ b/XFoil_Data.xlsx
@@ -24,15 +24,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
-  <si>
-    <t>alpha(deg)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>Cp</t>
+  </si>
+  <si>
+    <t>alpha(deg)_1</t>
+  </si>
+  <si>
+    <t>alpha(deg)_2</t>
+  </si>
+  <si>
+    <t>alpha(deg)_3</t>
+  </si>
+  <si>
+    <t>alpha(deg)_4</t>
+  </si>
+  <si>
+    <t>alpha(deg)_5</t>
+  </si>
+  <si>
+    <t>alpha(deg)_6</t>
   </si>
 </sst>
 </file>
@@ -392,8 +407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R251"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="K177" sqref="K177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,58 +423,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="J1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="M1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>2</v>
-      </c>
       <c r="P1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>1</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>